<commit_message>
feat: tables_config: pivot, datetime implemented
</commit_message>
<xml_diff>
--- a/src/yarm/tests_data/test_validate_complete_config_valid/SOURCE_A.xlsx
+++ b/src/yarm/tests_data/test_validate_complete_config_valid/SOURCE_A.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="A.2" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="A.DATETIME" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="A.1" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
@@ -21,15 +21,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+  <si>
+    <t xml:space="preserve">ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CREATED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MODIFIED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TOUCHED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A2.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A2.2</t>
+  </si>
   <si>
     <t xml:space="preserve">id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A2.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A2.2</t>
   </si>
   <si>
     <t xml:space="preserve">A1.1</t>
@@ -39,8 +51,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="mm/dd/yy"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -107,12 +120,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -133,27 +150,54 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="164" zoomScaleNormal="164" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="400" zoomScaleNormal="400" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>25934</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>25935</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>28858</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>29265</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>29297</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>36525</v>
       </c>
     </row>
   </sheetData>
@@ -174,25 +218,25 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="164" zoomScaleNormal="164" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="400" zoomScaleNormal="400" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
query options: replace: works, start on postprocess:
</commit_message>
<xml_diff>
--- a/src/yarm/tests_data/test_validate_complete_config_valid/SOURCE_A.xlsx
+++ b/src/yarm/tests_data/test_validate_complete_config_valid/SOURCE_A.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="A.DATETIME" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -44,7 +44,10 @@
     <t xml:space="preserve">id</t>
   </si>
   <si>
-    <t xml:space="preserve">A1.1</t>
+    <t xml:space="preserve">FIELD_A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MATCH A1</t>
   </si>
 </sst>
 </file>
@@ -152,11 +155,11 @@
   </sheetPr>
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="400" zoomScaleNormal="400" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="400" zoomScaleNormal="400" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -216,27 +219,36 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="400" zoomScaleNormal="400" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="400" zoomScaleNormal="400" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="B1" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>7</v>
+      <c r="A2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>7</v>
+      <c r="A3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
docs: options: output:, input:
</commit_message>
<xml_diff>
--- a/src/yarm/tests_data/test_validate_complete_config_valid/SOURCE_A.xlsx
+++ b/src/yarm/tests_data/test_validate_complete_config_valid/SOURCE_A.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="A.DATETIME" sheetId="1" state="visible" r:id="rId2"/>
@@ -44,7 +44,7 @@
     <t xml:space="preserve">id</t>
   </si>
   <si>
-    <t xml:space="preserve">FIELD_A</t>
+    <t xml:space="preserve">COLUMN_A</t>
   </si>
   <si>
     <t xml:space="preserve">MATCH A1</t>
@@ -155,11 +155,11 @@
   </sheetPr>
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="400" zoomScaleNormal="400" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="400" zoomScaleNormal="400" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -221,17 +221,17 @@
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="400" zoomScaleNormal="400" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="400" zoomScaleNormal="400" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
@@ -239,7 +239,7 @@
       <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
     </row>
@@ -247,7 +247,7 @@
       <c r="A3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>